<commit_message>
Add sample matching and fix datetimes with fractions of seconds
</commit_message>
<xml_diff>
--- a/data/Humphreys_peakform.xlsx
+++ b/data/Humphreys_peakform.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mphum\GitHub\koolstof\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067075DC-DC4A-40FB-B607-EBCBA94AE0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20666A1-89E6-41DD-9121-BE4FDE494977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A56CEC6-925E-4959-AEE1-9FEB0C105756}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>bottle</t>
   </si>
@@ -99,6 +99,72 @@
   </si>
   <si>
     <t>Junk_15</t>
+  </si>
+  <si>
+    <t>Junk2_00</t>
+  </si>
+  <si>
+    <t>Junk2_01</t>
+  </si>
+  <si>
+    <t>Junk2_02</t>
+  </si>
+  <si>
+    <t>Junk2_03</t>
+  </si>
+  <si>
+    <t>Junk2_04</t>
+  </si>
+  <si>
+    <t>Junk2_05</t>
+  </si>
+  <si>
+    <t>Junk2_06</t>
+  </si>
+  <si>
+    <t>Junk2_07</t>
+  </si>
+  <si>
+    <t>Junk2_08</t>
+  </si>
+  <si>
+    <t>Junk2_cal0_0</t>
+  </si>
+  <si>
+    <t>Junk2_cal1_0</t>
+  </si>
+  <si>
+    <t>Junk2_cal2_0</t>
+  </si>
+  <si>
+    <t>Junk2_cal3_0</t>
+  </si>
+  <si>
+    <t>Junk2_cal2_1</t>
+  </si>
+  <si>
+    <t>Junk2_cal4_0</t>
+  </si>
+  <si>
+    <t>aborted, volume too big?</t>
+  </si>
+  <si>
+    <t>Junk2_cal3_1</t>
+  </si>
+  <si>
+    <t>Junk2_cal1_1</t>
+  </si>
+  <si>
+    <t>Junk2_cal0_1</t>
+  </si>
+  <si>
+    <t>Junk2_09</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -128,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,12 +202,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,436 +537,1206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309EA9E0-FB5A-4A2F-9EB7-46C77111B268}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="M1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1500</v>
-      </c>
       <c r="C2">
-        <v>40</v>
+        <v>1500</v>
       </c>
       <c r="D2">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>150</v>
       </c>
       <c r="F2">
+        <v>150</v>
+      </c>
+      <c r="G2">
         <v>300</v>
       </c>
-      <c r="G2">
-        <v>40</v>
-      </c>
       <c r="H2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1000</v>
       </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
       <c r="D3">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>150</v>
       </c>
       <c r="F3">
+        <v>150</v>
+      </c>
+      <c r="G3">
         <v>300</v>
       </c>
-      <c r="G3">
-        <v>40</v>
-      </c>
       <c r="H3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>250</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>1500</v>
-      </c>
       <c r="C4">
-        <v>40</v>
+        <v>1500</v>
       </c>
       <c r="D4">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>150</v>
       </c>
       <c r="F4">
+        <v>150</v>
+      </c>
+      <c r="G4">
         <v>300</v>
       </c>
-      <c r="G4">
-        <v>40</v>
-      </c>
       <c r="H4">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>1500</v>
-      </c>
       <c r="C5">
-        <v>40</v>
+        <v>1500</v>
       </c>
       <c r="D5">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>150</v>
       </c>
       <c r="F5">
+        <v>150</v>
+      </c>
+      <c r="G5">
         <v>300</v>
       </c>
-      <c r="G5">
-        <v>40</v>
-      </c>
       <c r="H5">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>1500</v>
-      </c>
       <c r="C6">
-        <v>40</v>
+        <v>1500</v>
       </c>
       <c r="D6">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>150</v>
       </c>
       <c r="F6">
+        <v>150</v>
+      </c>
+      <c r="G6">
         <v>300</v>
       </c>
-      <c r="G6">
-        <v>40</v>
-      </c>
       <c r="H6">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
-        <v>1500</v>
-      </c>
       <c r="C7">
+        <v>1500</v>
+      </c>
+      <c r="D7">
         <v>20</v>
       </c>
-      <c r="D7">
-        <v>150</v>
-      </c>
       <c r="E7">
         <v>150</v>
       </c>
       <c r="F7">
+        <v>150</v>
+      </c>
+      <c r="G7">
         <v>300</v>
       </c>
-      <c r="G7">
-        <v>40</v>
-      </c>
       <c r="H7">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
-        <v>1500</v>
-      </c>
       <c r="C8">
+        <v>1500</v>
+      </c>
+      <c r="D8">
         <v>20</v>
       </c>
-      <c r="D8">
-        <v>150</v>
-      </c>
       <c r="E8">
         <v>150</v>
       </c>
       <c r="F8">
-        <v>360</v>
+        <v>150</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="H8">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
-        <v>1500</v>
-      </c>
       <c r="C9">
+        <v>1500</v>
+      </c>
+      <c r="D9">
         <v>20</v>
       </c>
-      <c r="D9">
-        <v>150</v>
-      </c>
       <c r="E9">
         <v>150</v>
       </c>
       <c r="F9">
-        <v>360</v>
+        <v>150</v>
       </c>
       <c r="G9">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="H9">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <v>1500</v>
-      </c>
       <c r="C10">
+        <v>1500</v>
+      </c>
+      <c r="D10">
         <v>30</v>
       </c>
-      <c r="D10">
-        <v>150</v>
-      </c>
       <c r="E10">
         <v>150</v>
       </c>
       <c r="F10">
-        <v>360</v>
+        <v>150</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="H10">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>1500</v>
-      </c>
       <c r="C11">
+        <v>1500</v>
+      </c>
+      <c r="D11">
         <v>30</v>
       </c>
-      <c r="D11">
-        <v>150</v>
-      </c>
       <c r="E11">
         <v>150</v>
       </c>
       <c r="F11">
-        <v>360</v>
+        <v>150</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="H11">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>44004</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>1500</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>150</v>
-      </c>
-      <c r="E12">
-        <v>150</v>
-      </c>
-      <c r="F12">
-        <v>360</v>
-      </c>
-      <c r="G12">
-        <v>40</v>
-      </c>
-      <c r="H12">
-        <v>120</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>100</v>
-      </c>
-      <c r="K12">
+      <c r="C12" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D12" s="1">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1">
+        <v>150</v>
+      </c>
+      <c r="F12" s="1">
+        <v>150</v>
+      </c>
+      <c r="G12" s="1">
+        <v>360</v>
+      </c>
+      <c r="H12" s="1">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1">
+        <v>120</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>100</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>1500</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>150</v>
+      </c>
+      <c r="F13">
+        <v>150</v>
+      </c>
+      <c r="G13">
+        <v>360</v>
+      </c>
+      <c r="H13">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <v>120</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>1500</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>150</v>
+      </c>
+      <c r="F14">
+        <v>150</v>
+      </c>
+      <c r="G14">
+        <v>360</v>
+      </c>
+      <c r="H14">
+        <v>40</v>
+      </c>
+      <c r="I14">
+        <v>120</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>1500</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>150</v>
+      </c>
+      <c r="F15">
+        <v>150</v>
+      </c>
+      <c r="G15">
+        <v>360</v>
+      </c>
+      <c r="H15">
+        <v>40</v>
+      </c>
+      <c r="I15">
+        <v>120</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>1500</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+      <c r="G16">
+        <v>360</v>
+      </c>
+      <c r="H16">
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <v>120</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <v>150</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+      <c r="G17">
+        <v>360</v>
+      </c>
+      <c r="H17">
+        <v>40</v>
+      </c>
+      <c r="I17">
+        <v>120</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>1500</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>150</v>
+      </c>
+      <c r="F18">
+        <v>150</v>
+      </c>
+      <c r="G18">
+        <v>360</v>
+      </c>
+      <c r="H18">
+        <v>40</v>
+      </c>
+      <c r="I18">
+        <v>120</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>1500</v>
+      </c>
+      <c r="D19">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>150</v>
+      </c>
+      <c r="F19">
+        <v>150</v>
+      </c>
+      <c r="G19">
+        <v>360</v>
+      </c>
+      <c r="H19">
+        <v>40</v>
+      </c>
+      <c r="I19">
+        <v>120</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>1500</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <v>150</v>
+      </c>
+      <c r="F20">
+        <v>150</v>
+      </c>
+      <c r="G20">
+        <v>360</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20">
+        <v>120</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>1500</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <v>150</v>
+      </c>
+      <c r="F21">
+        <v>150</v>
+      </c>
+      <c r="G21">
+        <v>360</v>
+      </c>
+      <c r="H21">
+        <v>40</v>
+      </c>
+      <c r="I21">
+        <v>120</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>500</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22">
+        <v>150</v>
+      </c>
+      <c r="F22">
+        <v>150</v>
+      </c>
+      <c r="G22">
+        <v>360</v>
+      </c>
+      <c r="H22">
+        <v>40</v>
+      </c>
+      <c r="I22">
+        <v>120</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>1000</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>150</v>
+      </c>
+      <c r="F23">
+        <v>150</v>
+      </c>
+      <c r="G23">
+        <v>360</v>
+      </c>
+      <c r="H23">
+        <v>40</v>
+      </c>
+      <c r="I23">
+        <v>120</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>100</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>1500</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>150</v>
+      </c>
+      <c r="F24">
+        <v>150</v>
+      </c>
+      <c r="G24">
+        <v>360</v>
+      </c>
+      <c r="H24">
+        <v>40</v>
+      </c>
+      <c r="I24">
+        <v>120</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>2000</v>
+      </c>
+      <c r="D25">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <v>150</v>
+      </c>
+      <c r="F25">
+        <v>150</v>
+      </c>
+      <c r="G25">
+        <v>360</v>
+      </c>
+      <c r="H25">
+        <v>40</v>
+      </c>
+      <c r="I25">
+        <v>120</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>100</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26">
+        <v>2500</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <v>150</v>
+      </c>
+      <c r="F26">
+        <v>150</v>
+      </c>
+      <c r="G26">
+        <v>360</v>
+      </c>
+      <c r="H26">
+        <v>40</v>
+      </c>
+      <c r="I26">
+        <v>120</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>100</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>2000</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <v>150</v>
+      </c>
+      <c r="F27">
+        <v>150</v>
+      </c>
+      <c r="G27">
+        <v>360</v>
+      </c>
+      <c r="H27">
+        <v>40</v>
+      </c>
+      <c r="I27">
+        <v>120</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>150</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>1500</v>
+      </c>
+      <c r="D28">
+        <v>50</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+      <c r="F28">
+        <v>150</v>
+      </c>
+      <c r="G28">
+        <v>360</v>
+      </c>
+      <c r="H28">
+        <v>40</v>
+      </c>
+      <c r="I28">
+        <v>120</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>150</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29">
+        <v>1000</v>
+      </c>
+      <c r="D29">
+        <v>50</v>
+      </c>
+      <c r="E29">
+        <v>150</v>
+      </c>
+      <c r="F29">
+        <v>150</v>
+      </c>
+      <c r="G29">
+        <v>360</v>
+      </c>
+      <c r="H29">
+        <v>40</v>
+      </c>
+      <c r="I29">
+        <v>120</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>150</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>500</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30">
+        <v>150</v>
+      </c>
+      <c r="F30">
+        <v>150</v>
+      </c>
+      <c r="G30">
+        <v>360</v>
+      </c>
+      <c r="H30">
+        <v>40</v>
+      </c>
+      <c r="I30">
+        <v>120</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>150</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>44008</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D31" s="1">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1">
+        <v>150</v>
+      </c>
+      <c r="F31" s="1">
+        <v>150</v>
+      </c>
+      <c r="G31" s="1">
+        <v>360</v>
+      </c>
+      <c r="H31" s="1">
+        <v>40</v>
+      </c>
+      <c r="I31" s="1">
+        <v>120</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>150</v>
+      </c>
+      <c r="L31" s="6">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Putting things together in the lab, not much progress
</commit_message>
<xml_diff>
--- a/data/Humphreys_peakform.xlsx
+++ b/data/Humphreys_peakform.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mphum\GitHub\koolstof\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93F80BA-DBDB-4416-9122-295B9A756B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02B9D25-2025-4483-AFC2-240F9EE8069A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4248" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{3A56CEC6-925E-4959-AEE1-9FEB0C105756}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A56CEC6-925E-4959-AEE1-9FEB0C105756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>bottle</t>
   </si>
@@ -165,6 +165,72 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Junk3_01</t>
+  </si>
+  <si>
+    <t>new acid added before this run</t>
+  </si>
+  <si>
+    <t>Junk3_02</t>
+  </si>
+  <si>
+    <t>Junk3_03</t>
+  </si>
+  <si>
+    <t>Junk3_04</t>
+  </si>
+  <si>
+    <t>maybe a tiny shoulder</t>
+  </si>
+  <si>
+    <t>Junk3_05</t>
+  </si>
+  <si>
+    <t>Junk3_06</t>
+  </si>
+  <si>
+    <t>Junk3_07</t>
+  </si>
+  <si>
+    <t>Junk3_08</t>
+  </si>
+  <si>
+    <t>extra NaHCO3</t>
+  </si>
+  <si>
+    <t>JunkHI_01</t>
+  </si>
+  <si>
+    <t>back to original junk</t>
+  </si>
+  <si>
+    <t>Junk3_09</t>
+  </si>
+  <si>
+    <t>Junk3_10</t>
+  </si>
+  <si>
+    <t>Junk3_11</t>
+  </si>
+  <si>
+    <t>Junk3_12</t>
+  </si>
+  <si>
+    <t>Junk3_13</t>
+  </si>
+  <si>
+    <t>Junk3_14</t>
+  </si>
+  <si>
+    <t>little delay sorting out software before this one</t>
+  </si>
+  <si>
+    <t>Junk3_15</t>
+  </si>
+  <si>
+    <t>Junk3_16</t>
   </si>
 </sst>
 </file>
@@ -537,11 +603,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309EA9E0-FB5A-4A2F-9EB7-46C77111B268}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,6 +1800,667 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D32" s="2">
+        <v>20</v>
+      </c>
+      <c r="E32" s="2">
+        <v>150</v>
+      </c>
+      <c r="F32" s="2">
+        <v>150</v>
+      </c>
+      <c r="G32" s="2">
+        <v>360</v>
+      </c>
+      <c r="H32" s="2">
+        <v>60</v>
+      </c>
+      <c r="I32" s="2">
+        <v>120</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>100</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D33" s="2">
+        <v>20</v>
+      </c>
+      <c r="E33" s="2">
+        <v>150</v>
+      </c>
+      <c r="F33" s="2">
+        <v>150</v>
+      </c>
+      <c r="G33" s="2">
+        <v>400</v>
+      </c>
+      <c r="H33" s="2">
+        <v>60</v>
+      </c>
+      <c r="I33" s="2">
+        <v>120</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>100</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D34" s="2">
+        <v>20</v>
+      </c>
+      <c r="E34" s="2">
+        <v>150</v>
+      </c>
+      <c r="F34" s="2">
+        <v>150</v>
+      </c>
+      <c r="G34" s="2">
+        <v>400</v>
+      </c>
+      <c r="H34" s="2">
+        <v>60</v>
+      </c>
+      <c r="I34" s="2">
+        <v>120</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>100</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1800</v>
+      </c>
+      <c r="D35" s="2">
+        <v>20</v>
+      </c>
+      <c r="E35" s="2">
+        <v>150</v>
+      </c>
+      <c r="F35" s="2">
+        <v>150</v>
+      </c>
+      <c r="G35" s="2">
+        <v>400</v>
+      </c>
+      <c r="H35" s="2">
+        <v>60</v>
+      </c>
+      <c r="I35" s="2">
+        <v>120</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>100</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2200</v>
+      </c>
+      <c r="D36" s="2">
+        <v>20</v>
+      </c>
+      <c r="E36" s="2">
+        <v>150</v>
+      </c>
+      <c r="F36" s="2">
+        <v>150</v>
+      </c>
+      <c r="G36" s="2">
+        <v>400</v>
+      </c>
+      <c r="H36" s="2">
+        <v>60</v>
+      </c>
+      <c r="I36" s="2">
+        <v>120</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>100</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1900</v>
+      </c>
+      <c r="D37" s="2">
+        <v>20</v>
+      </c>
+      <c r="E37" s="2">
+        <v>150</v>
+      </c>
+      <c r="F37" s="2">
+        <v>150</v>
+      </c>
+      <c r="G37" s="2">
+        <v>400</v>
+      </c>
+      <c r="H37" s="2">
+        <v>60</v>
+      </c>
+      <c r="I37" s="2">
+        <v>120</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>100</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2100</v>
+      </c>
+      <c r="D38" s="2">
+        <v>20</v>
+      </c>
+      <c r="E38" s="2">
+        <v>150</v>
+      </c>
+      <c r="F38" s="2">
+        <v>150</v>
+      </c>
+      <c r="G38" s="2">
+        <v>400</v>
+      </c>
+      <c r="H38" s="2">
+        <v>60</v>
+      </c>
+      <c r="I38" s="2">
+        <v>120</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>100</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D39" s="2">
+        <v>20</v>
+      </c>
+      <c r="E39" s="2">
+        <v>150</v>
+      </c>
+      <c r="F39" s="2">
+        <v>150</v>
+      </c>
+      <c r="G39" s="2">
+        <v>400</v>
+      </c>
+      <c r="H39" s="2">
+        <v>60</v>
+      </c>
+      <c r="I39" s="2">
+        <v>120</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>100</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D40" s="2">
+        <v>20</v>
+      </c>
+      <c r="E40" s="2">
+        <v>150</v>
+      </c>
+      <c r="F40" s="2">
+        <v>150</v>
+      </c>
+      <c r="G40" s="2">
+        <v>400</v>
+      </c>
+      <c r="H40" s="2">
+        <v>60</v>
+      </c>
+      <c r="I40" s="2">
+        <v>120</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>100</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D41" s="2">
+        <v>20</v>
+      </c>
+      <c r="E41" s="2">
+        <v>150</v>
+      </c>
+      <c r="F41" s="2">
+        <v>150</v>
+      </c>
+      <c r="G41" s="2">
+        <v>400</v>
+      </c>
+      <c r="H41" s="2">
+        <v>60</v>
+      </c>
+      <c r="I41" s="2">
+        <v>120</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>100</v>
+      </c>
+      <c r="L41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1800</v>
+      </c>
+      <c r="D42" s="2">
+        <v>18</v>
+      </c>
+      <c r="E42" s="2">
+        <v>150</v>
+      </c>
+      <c r="F42" s="2">
+        <v>150</v>
+      </c>
+      <c r="G42" s="2">
+        <v>400</v>
+      </c>
+      <c r="H42" s="2">
+        <v>60</v>
+      </c>
+      <c r="I42" s="2">
+        <v>120</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2">
+        <v>100</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2200</v>
+      </c>
+      <c r="D43" s="2">
+        <v>22</v>
+      </c>
+      <c r="E43" s="2">
+        <v>150</v>
+      </c>
+      <c r="F43" s="2">
+        <v>150</v>
+      </c>
+      <c r="G43" s="2">
+        <v>400</v>
+      </c>
+      <c r="H43" s="2">
+        <v>60</v>
+      </c>
+      <c r="I43" s="2">
+        <v>120</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2">
+        <v>100</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1900</v>
+      </c>
+      <c r="D44" s="2">
+        <v>19</v>
+      </c>
+      <c r="E44" s="2">
+        <v>150</v>
+      </c>
+      <c r="F44" s="2">
+        <v>150</v>
+      </c>
+      <c r="G44" s="2">
+        <v>400</v>
+      </c>
+      <c r="H44" s="2">
+        <v>60</v>
+      </c>
+      <c r="I44" s="2">
+        <v>120</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>100</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2100</v>
+      </c>
+      <c r="D45" s="2">
+        <v>21</v>
+      </c>
+      <c r="E45" s="2">
+        <v>150</v>
+      </c>
+      <c r="F45" s="2">
+        <v>150</v>
+      </c>
+      <c r="G45" s="2">
+        <v>400</v>
+      </c>
+      <c r="H45" s="2">
+        <v>60</v>
+      </c>
+      <c r="I45" s="2">
+        <v>120</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>100</v>
+      </c>
+      <c r="L45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D46" s="2">
+        <v>20</v>
+      </c>
+      <c r="E46" s="2">
+        <v>150</v>
+      </c>
+      <c r="F46" s="2">
+        <v>150</v>
+      </c>
+      <c r="G46" s="2">
+        <v>400</v>
+      </c>
+      <c r="H46" s="2">
+        <v>60</v>
+      </c>
+      <c r="I46" s="2">
+        <v>120</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>100</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D47" s="2">
+        <v>15</v>
+      </c>
+      <c r="E47" s="2">
+        <v>150</v>
+      </c>
+      <c r="F47" s="2">
+        <v>150</v>
+      </c>
+      <c r="G47" s="2">
+        <v>400</v>
+      </c>
+      <c r="H47" s="2">
+        <v>60</v>
+      </c>
+      <c r="I47" s="2">
+        <v>120</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>100</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>44011</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D48" s="2">
+        <v>20</v>
+      </c>
+      <c r="E48" s="2">
+        <v>150</v>
+      </c>
+      <c r="F48" s="2">
+        <v>150</v>
+      </c>
+      <c r="G48" s="2">
+        <v>400</v>
+      </c>
+      <c r="H48" s="2">
+        <v>60</v>
+      </c>
+      <c r="I48" s="2">
+        <v>120</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2">
+        <v>100</v>
+      </c>
+      <c r="L48" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New data and towards DIC calculation
</commit_message>
<xml_diff>
--- a/data/Humphreys_peakform.xlsx
+++ b/data/Humphreys_peakform.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mphum\GitHub\koolstof\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F79808-FA48-4A23-9DD7-7623853AC57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4CEE73-C4F9-4B3C-BABF-A084E3F1B84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A56CEC6-925E-4959-AEE1-9FEB0C105756}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>bottle</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Junk_20200703_09</t>
   </si>
   <si>
-    <t>Junk_20200703_10</t>
-  </si>
-  <si>
     <t>no sample delivered to stripper?</t>
   </si>
   <si>
@@ -294,6 +291,21 @@
   </si>
   <si>
     <t>Junk20200706_06</t>
+  </si>
+  <si>
+    <t>Junk20200706_07</t>
+  </si>
+  <si>
+    <t>Junk20200706_08</t>
+  </si>
+  <si>
+    <t>Junk20200706_09</t>
+  </si>
+  <si>
+    <t>Junk20200706_10</t>
+  </si>
+  <si>
+    <t>Junk_20200703_010</t>
   </si>
 </sst>
 </file>
@@ -666,11 +678,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309EA9E0-FB5A-4A2F-9EB7-46C77111B268}">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2831,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="M56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -2872,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="M57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2880,7 +2892,7 @@
         <v>44015</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C58" s="6">
         <v>2300</v>
@@ -2913,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -2921,7 +2933,7 @@
         <v>44015</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C59" s="2">
         <v>2300</v>
@@ -2954,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2962,7 +2974,7 @@
         <v>44015</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" s="6">
         <v>2300</v>
@@ -3000,7 +3012,7 @@
         <v>44018</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" s="2">
         <v>2000</v>
@@ -3038,7 +3050,7 @@
         <v>44018</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" s="2">
         <v>2000</v>
@@ -3076,7 +3088,7 @@
         <v>44018</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" s="2">
         <v>500</v>
@@ -3114,7 +3126,7 @@
         <v>44018</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="2">
         <v>1000</v>
@@ -3152,7 +3164,7 @@
         <v>44018</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" s="2">
         <v>1500</v>
@@ -3190,7 +3202,7 @@
         <v>44018</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" s="2">
         <v>2300</v>
@@ -3220,6 +3232,134 @@
         <v>150</v>
       </c>
       <c r="L66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <v>44018</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" s="2">
+        <v>150</v>
+      </c>
+      <c r="F67" s="2">
+        <v>150</v>
+      </c>
+      <c r="G67" s="2">
+        <v>400</v>
+      </c>
+      <c r="H67" s="2">
+        <v>60</v>
+      </c>
+      <c r="I67" s="2">
+        <v>120</v>
+      </c>
+      <c r="J67" s="2">
+        <v>0</v>
+      </c>
+      <c r="K67" s="2">
+        <v>150</v>
+      </c>
+      <c r="L67" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
+        <v>44018</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68" s="2">
+        <v>150</v>
+      </c>
+      <c r="F68" s="2">
+        <v>150</v>
+      </c>
+      <c r="G68" s="2">
+        <v>400</v>
+      </c>
+      <c r="H68" s="2">
+        <v>60</v>
+      </c>
+      <c r="I68" s="2">
+        <v>120</v>
+      </c>
+      <c r="J68" s="2">
+        <v>0</v>
+      </c>
+      <c r="K68" s="2">
+        <v>150</v>
+      </c>
+      <c r="L68" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <v>44018</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E69" s="2">
+        <v>150</v>
+      </c>
+      <c r="F69" s="2">
+        <v>150</v>
+      </c>
+      <c r="G69" s="2">
+        <v>400</v>
+      </c>
+      <c r="H69" s="2">
+        <v>60</v>
+      </c>
+      <c r="I69" s="2">
+        <v>120</v>
+      </c>
+      <c r="J69" s="2">
+        <v>0</v>
+      </c>
+      <c r="K69" s="2">
+        <v>150</v>
+      </c>
+      <c r="L69" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="5">
+        <v>44018</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E70" s="2">
+        <v>150</v>
+      </c>
+      <c r="F70" s="2">
+        <v>150</v>
+      </c>
+      <c r="G70" s="2">
+        <v>400</v>
+      </c>
+      <c r="H70" s="2">
+        <v>60</v>
+      </c>
+      <c r="I70" s="2">
+        <v>120</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0</v>
+      </c>
+      <c r="K70" s="2">
+        <v>150</v>
+      </c>
+      <c r="L70" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>